<commit_message>
add xlsx and xlsb version of issues
</commit_message>
<xml_diff>
--- a/tests/issues.xlsx
+++ b/tests/issues.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
   </bookViews>
   <sheets>
-    <sheet name="issue2" sheetId="1" r:id="rId1"/>
-    <sheet name="issue5" sheetId="2" r:id="rId2"/>
-    <sheet name="issue6" sheetId="3" r:id="rId3"/>
+    <sheet name="datatypes" sheetId="4" r:id="rId1"/>
+    <sheet name="issue2" sheetId="1" r:id="rId2"/>
+    <sheet name="issue5" sheetId="2" r:id="rId3"/>
+    <sheet name="issue6" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>a</t>
   </si>
@@ -25,6 +26,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -60,9 +64,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,6 +362,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="str">
+        <f>CONCATENATE("a","b")</f>
+        <v>ab</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="b">
+        <f>A1&gt;A2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2">
+        <v>42663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -394,12 +449,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -415,15 +470,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
@@ -447,6 +505,9 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test cases for specials characters
</commit_message>
<xml_diff>
--- a/tests/issues.xlsx
+++ b/tests/issues.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="datatypes" sheetId="4" r:id="rId1"/>
     <sheet name="issue2" sheetId="1" r:id="rId2"/>
     <sheet name="issue5" sheetId="2" r:id="rId3"/>
     <sheet name="issue6" sheetId="3" r:id="rId4"/>
+    <sheet name="spc_chrs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>a</t>
   </si>
@@ -29,19 +30,53 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>aaa ' aaa</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>☺</t>
+  </si>
+  <si>
+    <t>֍</t>
+  </si>
+  <si>
+    <t>àâéêèçöïî«»</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="U2400"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="U0400"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,10 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,13 +401,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -480,7 +517,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -511,4 +548,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add PtgRef3d and PtgRefErr3d
</commit_message>
<xml_diff>
--- a/tests/issues.xlsx
+++ b/tests/issues.xlsx
@@ -22,6 +22,7 @@
   <definedNames>
     <definedName name="MyBrokenRange">Sheet1!#REF!</definedName>
     <definedName name="MyDataTypes">datatypes!$A$1:$A$6</definedName>
+    <definedName name="OneRange">Sheet1!$A$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -505,9 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>